<commit_message>
Updated list pf planets which need to be modeled
</commit_message>
<xml_diff>
--- a/Design Documents/Planets to model/Planets to model.xlsx
+++ b/Design Documents/Planets to model/Planets to model.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Games\Documents\GitHub\level-6-l6-group-3\Design Documents\Planets to model\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Planet names </t>
   </si>
@@ -24,9 +29,6 @@
     <t xml:space="preserve">Rocky Planet </t>
   </si>
   <si>
-    <t xml:space="preserve">Antartic Planet </t>
-  </si>
-  <si>
     <t xml:space="preserve">Terra Planet </t>
   </si>
   <si>
@@ -39,9 +41,6 @@
     <t xml:space="preserve">Ice Planet </t>
   </si>
   <si>
-    <t xml:space="preserve">Industrial - Winter Planet </t>
-  </si>
-  <si>
     <t xml:space="preserve">Crystal Planet </t>
   </si>
   <si>
@@ -51,9 +50,6 @@
     <t xml:space="preserve">Metalic - Earth like Planet </t>
   </si>
   <si>
-    <t xml:space="preserve">Earth-Gold Planet </t>
-  </si>
-  <si>
     <t xml:space="preserve">Nickel Planet </t>
   </si>
   <si>
@@ -61,12 +57,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fluid Metal Planet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gold like Industrial Planet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metalic Gold Planet </t>
   </si>
   <si>
     <t>Completed</t>
@@ -78,8 +68,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +122,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -178,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,9 +208,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,6 +260,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,28 +453,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H15:H16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -448,133 +482,113 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B18">
@@ -592,24 +606,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>